<commit_message>
Drugi plecka i menu
</commit_message>
<xml_diff>
--- a/sdizo3/wyniki_plecak.xlsx
+++ b/sdizo3/wyniki_plecak.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Damian\Na Studia\Studia\SDiZO\Projekt\Projekt3\Plecak\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Damian\Na Studia\Studia\SDiZO\Projekt\Projekt3\GIT\sdizo3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="N=1000" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="N=10000" sheetId="3" r:id="rId3"/>
     <sheet name="N=20000" sheetId="4" r:id="rId4"/>
     <sheet name="N=50000" sheetId="5" r:id="rId5"/>
+    <sheet name="Arkusz1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>N=1000</t>
   </si>
@@ -61,6 +62,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>N=13</t>
+  </si>
+  <si>
+    <t>N=5</t>
   </si>
 </sst>
 </file>
@@ -148,7 +155,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -865,11 +871,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228813376"/>
-        <c:axId val="229688240"/>
+        <c:axId val="246840352"/>
+        <c:axId val="246840912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228813376"/>
+        <c:axId val="246840352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -926,12 +932,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229688240"/>
+        <c:crossAx val="246840912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229688240"/>
+        <c:axId val="246840912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -988,7 +994,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228813376"/>
+        <c:crossAx val="246840352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1194,11 +1200,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="313064144"/>
-        <c:axId val="313063584"/>
+        <c:axId val="246843152"/>
+        <c:axId val="246843712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="313064144"/>
+        <c:axId val="246843152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,7 +1308,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313063584"/>
+        <c:crossAx val="246843712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1310,7 +1316,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="313063584"/>
+        <c:axId val="246843712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1417,7 +1423,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313064144"/>
+        <c:crossAx val="246843152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1655,11 +1661,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="322817168"/>
-        <c:axId val="322817728"/>
+        <c:axId val="246845952"/>
+        <c:axId val="246846512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="322817168"/>
+        <c:axId val="246845952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +1769,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322817728"/>
+        <c:crossAx val="246846512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1771,7 +1777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322817728"/>
+        <c:axId val="246846512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1878,7 +1884,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322817168"/>
+        <c:crossAx val="246845952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2116,11 +2122,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="318499392"/>
-        <c:axId val="322863520"/>
+        <c:axId val="250431024"/>
+        <c:axId val="250431584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="318499392"/>
+        <c:axId val="250431024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,7 +2230,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322863520"/>
+        <c:crossAx val="250431584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2232,7 +2238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322863520"/>
+        <c:axId val="250431584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2339,7 +2345,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318499392"/>
+        <c:crossAx val="250431024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2889,11 +2895,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228061104"/>
-        <c:axId val="228061664"/>
+        <c:axId val="250436064"/>
+        <c:axId val="250436624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228061104"/>
+        <c:axId val="250436064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3011,12 +3017,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228061664"/>
+        <c:crossAx val="250436624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="228061664"/>
+        <c:axId val="250436624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3129,7 +3135,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228061104"/>
+        <c:crossAx val="250436064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6414,7 +6420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:L5"/>
     </sheetView>
   </sheetViews>
@@ -9350,4 +9356,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6.8557599999999996E-2</v>
+      </c>
+      <c r="D3">
+        <v>1757.2175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>